<commit_message>
+ Update code to read summary test case to get test case setting
</commit_message>
<xml_diff>
--- a/data/test_case_define.xlsx
+++ b/data/test_case_define.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sites\LearnAutomationTest\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7248" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7248"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="79">
   <si>
     <t>Step ID</t>
   </si>
@@ -212,18 +212,6 @@
     <t>btnG</t>
   </si>
   <si>
-    <t>TEST_ID</t>
-  </si>
-  <si>
-    <t>Browse</t>
-  </si>
-  <si>
-    <t>Test_Type</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
     <t>test001</t>
   </si>
   <si>
@@ -255,6 +243,27 @@
   </si>
   <si>
     <t>my-page</t>
+  </si>
+  <si>
+    <t>test_id</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>browser_type</t>
+  </si>
+  <si>
+    <t>test_type</t>
+  </si>
+  <si>
+    <t>test003</t>
+  </si>
+  <si>
+    <t>Test something</t>
+  </si>
+  <si>
+    <t>manual</t>
   </si>
 </sst>
 </file>
@@ -584,10 +593,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -597,61 +607,75 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="E1" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
         <v>68</v>
-      </c>
-      <c r="C2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="s">
         <v>67</v>
       </c>
-      <c r="B4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" t="s">
-        <v>71</v>
-      </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -661,6 +685,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -832,13 +857,13 @@
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D8" t="s">
         <v>42</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F8" t="s">
         <v>28</v>
@@ -880,9 +905,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1019,7 +1045,7 @@
         <v>28</v>
       </c>
       <c r="H6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -1035,6 +1061,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">

</xml_diff>